<commit_message>
03/04 - Presentation information for Sprint 2
</commit_message>
<xml_diff>
--- a/Modelling/2023_Betting_Prediction.xlsx
+++ b/Modelling/2023_Betting_Prediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c4038fad9741b6e/BrainStation/Data_Science_Bootcamp/Capstone_Project/capstone-Aboard89/Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A69C64A-219A-417A-B3AB-E017499A81AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{9A69C64A-219A-417A-B3AB-E017499A81AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8A45E81-D95C-438A-865D-D9E72DBD44FB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF633AC3-A18A-4EDB-BAA2-6048CA558DB4}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -748,7 +748,7 @@
       <name val="__titillium_0cbd66"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,6 +776,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -838,8 +844,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11148,7 +11154,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1DA74F64-AACC-45D0-948C-52805BAF3562}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1DA74F64-AACC-45D0-948C-52805BAF3562}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="40">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -11617,7 +11623,7 @@
   <dimension ref="A2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11630,22 +11636,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
-      <c r="A2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="12"/>
@@ -11660,13 +11666,13 @@
       <c r="B3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F3" s="14">
@@ -11684,13 +11690,13 @@
       <c r="B4" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F4" s="12">
@@ -11708,13 +11714,13 @@
       <c r="B5" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F5" s="12">
@@ -11732,13 +11738,13 @@
       <c r="B6" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F6" s="12">
@@ -11756,13 +11762,13 @@
       <c r="B7" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="12">
@@ -11780,13 +11786,13 @@
       <c r="B8" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F8" s="12">
@@ -11804,13 +11810,13 @@
       <c r="B9" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F9" s="12">
@@ -11828,13 +11834,13 @@
       <c r="B10" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F10" s="12">
@@ -11852,13 +11858,13 @@
       <c r="B11" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="12">
@@ -11876,13 +11882,13 @@
       <c r="B12" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F12" s="12">
@@ -11900,13 +11906,13 @@
       <c r="B13" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="12">
@@ -11924,13 +11930,13 @@
       <c r="B14" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F14" s="12">

</xml_diff>

<commit_message>
14/04 - Final Notebook Cleanups (e.g. formatting, spell checks, table of contents, introductions, conclusions, images, etc)
</commit_message>
<xml_diff>
--- a/Modelling/2023_Betting_Prediction.xlsx
+++ b/Modelling/2023_Betting_Prediction.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c4038fad9741b6e/BrainStation/Data_Science_Bootcamp/Capstone_Project/capstone-Aboard89/Modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{9A69C64A-219A-417A-B3AB-E017499A81AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8A45E81-D95C-438A-865D-D9E72DBD44FB}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{9A69C64A-219A-417A-B3AB-E017499A81AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF282C26-9106-4D58-9355-22132C05779F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF633AC3-A18A-4EDB-BAA2-6048CA558DB4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="10" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2890" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2906" uniqueCount="214">
   <si>
     <t>Race</t>
   </si>
@@ -681,6 +682,9 @@
   <si>
     <t>Team</t>
   </si>
+  <si>
+    <t>Japanese Grand Prix</t>
+  </si>
 </sst>
 </file>
 
@@ -863,6 +867,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Alex" refreshedDate="45377.80280208333" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="241" xr:uid="{DC1A99F8-5CF2-48E2-B00C-9BD4B5930FB0}">
   <cacheSource type="worksheet">
@@ -11154,7 +11162,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1DA74F64-AACC-45D0-948C-52805BAF3562}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1DA74F64-AACC-45D0-948C-52805BAF3562}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="40">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -11619,11 +11627,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248CAD67-FC4F-4BDF-A759-5FA20FF9FD59}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4D121F-0AB5-4F60-8DA8-D960E2B0FEED}">
   <dimension ref="A2:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12012,7 +12100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764A1B19-741C-4692-BA76-5B3FEC57A2B6}">
   <dimension ref="A3:B16"/>
   <sheetViews>
@@ -12143,7 +12231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A707FAB-2591-47A0-B41A-7CF0354BBEC4}">
   <dimension ref="A1:AN241"/>
   <sheetViews>

</xml_diff>